<commit_message>
dev of use items
</commit_message>
<xml_diff>
--- a/gameData/shared/Items.xlsx
+++ b/gameData/shared/Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="21640" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="6780" yWindow="21820" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="special" sheetId="2" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>movingConstruction </t>
-  </si>
-  <si>
     <t>torch</t>
   </si>
   <si>
@@ -633,6 +630,10 @@
   </si>
   <si>
     <t>dragonMaterials:ingo_3:5:12,dragonMaterials:redSoul_3:5:10,dragonMaterials:blueSoul_3:5:10,dragonMaterials:greenSoul_3:5:10,dragonMaterials:redCrystal_3:5:11,dragonMaterials:blueCrystal_3:5:11,dragonMaterials:greenCrystal_3:5:11,dragonMaterials:runes_3:5:11,dragonMaterials:ingo_4:2:1,dragonMaterials:redSoul_4:2:2,dragonMaterials:blueSoul_4:2:2,dragonMaterials:greenSoul_4:2:2,dragonMaterials:redCrystal_4:2:2,dragonMaterials:blueCrystal_4:2:2,dragonMaterials:greenCrystal_4:2:2,dragonMaterials:runes_4:2:1</t>
+  </si>
+  <si>
+    <t>movingConstruction</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -788,7 +789,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="162">
+  <cellStyleXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -803,6 +804,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -986,7 +991,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="162">
+  <cellStyles count="166">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1070,6 +1075,8 @@
     <cellStyle name="超链接" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="158" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="164" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1146,6 +1153,8 @@
     <cellStyle name="访问过的超链接" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="159" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="165" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1597,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -1617,42 +1626,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>1</v>
+        <v>185</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1">
         <v>200</v>
@@ -1660,22 +1669,22 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1">
         <v>200</v>
@@ -1683,22 +1692,22 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="1">
         <v>200</v>
@@ -1706,22 +1715,22 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1">
         <v>200</v>
@@ -1729,22 +1738,22 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" s="1">
         <v>200</v>
@@ -1752,22 +1761,22 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1">
         <v>200</v>
@@ -1775,7 +1784,7 @@
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7">
         <v>100</v>
@@ -1784,13 +1793,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1">
         <v>200</v>
@@ -1798,7 +1807,7 @@
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7">
         <v>500</v>
@@ -1807,13 +1816,13 @@
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="1">
         <v>200</v>
@@ -1821,7 +1830,7 @@
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7">
         <v>1000</v>
@@ -1830,13 +1839,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1">
         <v>200</v>
@@ -1844,7 +1853,7 @@
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="7">
         <v>100</v>
@@ -1853,13 +1862,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1">
         <v>200</v>
@@ -1867,7 +1876,7 @@
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7">
         <v>500</v>
@@ -1876,13 +1885,13 @@
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="1">
         <v>200</v>
@@ -1890,7 +1899,7 @@
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7">
         <v>1000</v>
@@ -1899,13 +1908,13 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1">
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1">
         <v>200</v>
@@ -1913,7 +1922,7 @@
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7">
         <v>100</v>
@@ -1922,13 +1931,13 @@
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="1">
         <v>200</v>
@@ -1936,7 +1945,7 @@
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7">
         <v>500</v>
@@ -1945,13 +1954,13 @@
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1">
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="1">
         <v>200</v>
@@ -1959,7 +1968,7 @@
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="7">
         <v>1000</v>
@@ -1968,13 +1977,13 @@
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1">
         <v>10</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="1">
         <v>200</v>
@@ -1982,7 +1991,7 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7">
         <v>20</v>
@@ -1991,13 +2000,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1">
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" s="1">
         <v>200</v>
@@ -2005,7 +2014,7 @@
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7">
         <v>50</v>
@@ -2014,13 +2023,13 @@
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="1">
         <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1">
         <v>200</v>
@@ -2028,7 +2037,7 @@
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="7">
         <v>100</v>
@@ -2037,13 +2046,13 @@
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1">
         <v>10</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="1">
         <v>200</v>
@@ -2051,7 +2060,7 @@
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7">
         <v>100</v>
@@ -2060,13 +2069,13 @@
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="1">
         <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G20" s="1">
         <v>200</v>
@@ -2074,7 +2083,7 @@
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="7">
         <v>500</v>
@@ -2083,13 +2092,13 @@
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="1">
         <v>10</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="1">
         <v>200</v>
@@ -2097,7 +2106,7 @@
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7">
         <v>1000</v>
@@ -2106,13 +2115,13 @@
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1">
         <v>10</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="1">
         <v>200</v>
@@ -2120,22 +2129,22 @@
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" s="2">
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="1">
         <v>10</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G23" s="1">
         <v>200</v>
@@ -2143,22 +2152,22 @@
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C24" s="1">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1">
         <v>10</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G24" s="1">
         <v>200</v>
@@ -2166,22 +2175,22 @@
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C25" s="1">
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1">
         <v>10</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="1">
         <v>200</v>
@@ -2189,22 +2198,22 @@
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C26" s="2">
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="1">
         <v>10</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G26" s="1">
         <v>200</v>
@@ -2212,22 +2221,22 @@
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C27" s="1">
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="1">
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="1">
         <v>200</v>
@@ -2235,22 +2244,22 @@
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="1">
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="1">
         <v>200</v>
@@ -2258,22 +2267,22 @@
     </row>
     <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C29" s="2">
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1">
         <v>10</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G29" s="1">
         <v>200</v>
@@ -2281,22 +2290,22 @@
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="1">
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="1">
         <v>10</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" s="1">
         <v>200</v>
@@ -2304,22 +2313,22 @@
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1">
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="1">
         <v>10</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31" s="1">
         <v>200</v>
@@ -2327,22 +2336,22 @@
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="2">
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" s="1">
         <v>10</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G32" s="1">
         <v>200</v>
@@ -2350,7 +2359,7 @@
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="7">
         <v>30</v>
@@ -2359,13 +2368,13 @@
         <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E33" s="1">
         <v>10</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="1">
         <v>200</v>
@@ -2373,7 +2382,7 @@
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="7">
         <v>60</v>
@@ -2382,13 +2391,13 @@
         <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="1">
         <v>10</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G34" s="1">
         <v>200</v>
@@ -2396,7 +2405,7 @@
     </row>
     <row r="35" spans="1:7" ht="20" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" s="7">
         <v>1440</v>
@@ -2405,13 +2414,13 @@
         <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="1">
+        <v>10</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="E35" s="1">
-        <v>10</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G35" s="1">
         <v>200</v>
@@ -2419,7 +2428,7 @@
     </row>
     <row r="36" spans="1:7" ht="20" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="7">
         <v>10080</v>
@@ -2428,13 +2437,13 @@
         <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="1">
         <v>10</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G36" s="1">
         <v>200</v>
@@ -2442,7 +2451,7 @@
     </row>
     <row r="37" spans="1:7" ht="20" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="7">
         <v>43200</v>
@@ -2451,13 +2460,13 @@
         <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="1">
         <v>10</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G37" s="1">
         <v>200</v>
@@ -2465,7 +2474,7 @@
     </row>
     <row r="38" spans="1:7" ht="20" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="7">
         <v>100</v>
@@ -2474,13 +2483,13 @@
         <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="1">
+        <v>10</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="E38" s="1">
-        <v>10</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="G38" s="1">
         <v>200</v>
@@ -2488,7 +2497,7 @@
     </row>
     <row r="39" spans="1:7" ht="20" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="7">
         <v>300</v>
@@ -2497,13 +2506,13 @@
         <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="1">
         <v>10</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G39" s="1">
         <v>200</v>
@@ -2511,7 +2520,7 @@
     </row>
     <row r="40" spans="1:7" ht="20" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="7">
         <v>1000</v>
@@ -2520,13 +2529,13 @@
         <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="1">
         <v>10</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G40" s="1">
         <v>200</v>
@@ -2534,7 +2543,7 @@
     </row>
     <row r="41" spans="1:7" ht="20" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="7">
         <v>5000</v>
@@ -2543,13 +2552,13 @@
         <v>40</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="1">
         <v>10</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G41" s="1">
         <v>200</v>
@@ -2589,42 +2598,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1">
         <v>200</v>
@@ -2632,22 +2641,22 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1">
         <v>200</v>
@@ -2655,22 +2664,22 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="1">
         <v>200</v>
@@ -2678,22 +2687,22 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G5" s="1">
         <v>200</v>
@@ -2701,22 +2710,22 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="1">
         <v>200</v>
@@ -2724,22 +2733,22 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="1">
         <v>200</v>
@@ -2747,22 +2756,22 @@
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" s="1">
         <v>200</v>
@@ -2770,22 +2779,22 @@
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="1">
         <v>200</v>
@@ -2793,22 +2802,22 @@
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1">
         <v>200</v>
@@ -2816,22 +2825,22 @@
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G11" s="1">
         <v>200</v>
@@ -2839,22 +2848,22 @@
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="1">
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1">
         <v>200</v>
@@ -2862,22 +2871,22 @@
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1">
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1">
         <v>200</v>
@@ -2885,22 +2894,22 @@
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="2">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G14" s="1">
         <v>200</v>
@@ -2908,22 +2917,22 @@
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="1">
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="1">
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="1">
         <v>200</v>
@@ -2931,22 +2940,22 @@
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="1">
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1">
         <v>10</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G16" s="1">
         <v>200</v>
@@ -2954,22 +2963,22 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2">
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="1">
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" s="1">
         <v>200</v>
@@ -2977,22 +2986,22 @@
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1">
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="1">
         <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G18" s="1">
         <v>200</v>
@@ -3000,22 +3009,22 @@
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="1">
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="1">
         <v>10</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G19" s="1">
         <v>200</v>
@@ -3023,22 +3032,22 @@
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C20" s="2">
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="1">
         <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" s="1">
         <v>200</v>
@@ -3046,22 +3055,22 @@
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" s="1">
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E21" s="1">
         <v>10</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G21" s="1">
         <v>200</v>
@@ -3069,22 +3078,22 @@
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="1">
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1">
         <v>10</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" s="1">
         <v>200</v>
@@ -3092,22 +3101,22 @@
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="2">
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="1">
         <v>10</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G23" s="1">
         <v>200</v>
@@ -3115,22 +3124,22 @@
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" s="1">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1">
         <v>10</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" s="1">
         <v>200</v>
@@ -3138,22 +3147,22 @@
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C25" s="1">
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1">
         <v>10</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="1">
         <v>200</v>
@@ -3161,22 +3170,22 @@
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2">
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="1">
         <v>10</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G26" s="1">
         <v>200</v>
@@ -3184,22 +3193,22 @@
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C27" s="1">
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="1">
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="1">
         <v>200</v>
@@ -3207,22 +3216,22 @@
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="1">
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="1">
         <v>200</v>
@@ -3230,22 +3239,22 @@
     </row>
     <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C29" s="2">
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1">
         <v>10</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G29" s="1">
         <v>200</v>
@@ -3253,22 +3262,22 @@
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C30" s="1">
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" s="1">
         <v>10</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G30" s="1">
         <v>200</v>
@@ -3276,22 +3285,22 @@
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C31" s="1">
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E31" s="1">
         <v>10</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31" s="1">
         <v>200</v>
@@ -3299,22 +3308,22 @@
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C32" s="2">
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E32" s="1">
         <v>10</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G32" s="1">
         <v>200</v>
@@ -3322,22 +3331,22 @@
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1">
         <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E33" s="1">
         <v>10</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G33" s="1">
         <v>200</v>
@@ -3345,22 +3354,22 @@
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" s="1">
         <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="1">
         <v>10</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G34" s="1">
         <v>200</v>
@@ -3368,22 +3377,22 @@
     </row>
     <row r="35" spans="1:7" ht="20" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C35" s="2">
         <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E35" s="1">
         <v>10</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G35" s="1">
         <v>200</v>
@@ -3391,22 +3400,22 @@
     </row>
     <row r="36" spans="1:7" ht="20" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C36" s="1">
         <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="1">
         <v>10</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G36" s="1">
         <v>200</v>
@@ -3414,22 +3423,22 @@
     </row>
     <row r="37" spans="1:7" ht="20" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1">
         <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="1">
         <v>10</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G37" s="1">
         <v>200</v>
@@ -3437,22 +3446,22 @@
     </row>
     <row r="38" spans="1:7" ht="20" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C38" s="2">
         <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E38" s="1">
         <v>10</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G38" s="1">
         <v>200</v>
@@ -3460,22 +3469,22 @@
     </row>
     <row r="39" spans="1:7" ht="20" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1">
         <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="1">
         <v>10</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G39" s="1">
         <v>200</v>
@@ -3483,22 +3492,22 @@
     </row>
     <row r="40" spans="1:7" ht="20" customHeight="1">
       <c r="A40" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C40" s="1">
         <v>39</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E40" s="1">
         <v>10</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G40" s="1">
         <v>200</v>
@@ -3506,22 +3515,22 @@
     </row>
     <row r="41" spans="1:7" ht="20" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="2">
         <v>40</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E41" s="1">
         <v>10</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G41" s="1">
         <v>200</v>
@@ -3529,22 +3538,22 @@
     </row>
     <row r="42" spans="1:7" ht="20" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C42" s="1">
         <v>41</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="1">
         <v>10</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G42" s="1">
         <v>200</v>
@@ -3552,22 +3561,22 @@
     </row>
     <row r="43" spans="1:7" ht="20" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43" s="1">
         <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="1">
         <v>10</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G43" s="1">
         <v>200</v>
@@ -3575,22 +3584,22 @@
     </row>
     <row r="44" spans="1:7" ht="20" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="2">
         <v>43</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44" s="1">
         <v>10</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G44" s="1">
         <v>200</v>
@@ -3598,22 +3607,22 @@
     </row>
     <row r="45" spans="1:7" ht="20" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="1">
         <v>44</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E45" s="1">
         <v>10</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G45" s="1">
         <v>200</v>
@@ -3621,22 +3630,22 @@
     </row>
     <row r="46" spans="1:7" ht="20" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" s="1">
         <v>45</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E46" s="1">
         <v>10</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G46" s="1">
         <v>200</v>
@@ -3644,22 +3653,22 @@
     </row>
     <row r="47" spans="1:7" ht="20" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" s="2">
         <v>46</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="1">
         <v>10</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G47" s="1">
         <v>200</v>
@@ -3667,22 +3676,22 @@
     </row>
     <row r="48" spans="1:7" ht="20" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C48" s="1">
         <v>47</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E48" s="1">
         <v>10</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G48" s="1">
         <v>200</v>
@@ -3690,22 +3699,22 @@
     </row>
     <row r="49" spans="1:7" ht="20" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C49" s="1">
         <v>48</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E49" s="1">
         <v>10</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G49" s="1">
         <v>200</v>
@@ -3713,22 +3722,22 @@
     </row>
     <row r="50" spans="1:7" ht="20" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" s="2">
         <v>49</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E50" s="1">
         <v>10</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G50" s="1">
         <v>200</v>
@@ -3736,22 +3745,22 @@
     </row>
     <row r="51" spans="1:7" ht="20" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" s="1">
         <v>50</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E51" s="1">
         <v>10</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G51" s="1">
         <v>200</v>
@@ -3759,22 +3768,22 @@
     </row>
     <row r="52" spans="1:7" ht="20" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C52" s="1">
         <v>51</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E52" s="1">
         <v>10</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G52" s="1">
         <v>200</v>
@@ -3782,22 +3791,22 @@
     </row>
     <row r="53" spans="1:7" ht="20" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C53" s="2">
         <v>52</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E53" s="1">
         <v>10</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G53" s="1">
         <v>200</v>
@@ -3805,22 +3814,22 @@
     </row>
     <row r="54" spans="1:7" ht="20" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C54" s="1">
         <v>53</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E54" s="1">
         <v>10</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G54" s="1">
         <v>200</v>
@@ -3828,22 +3837,22 @@
     </row>
     <row r="55" spans="1:7" ht="20" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C55" s="1">
         <v>54</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E55" s="1">
         <v>10</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G55" s="1">
         <v>200</v>
@@ -3883,27 +3892,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1">
         <v>0.1</v>
@@ -3912,13 +3921,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1">
         <v>200</v>
@@ -3926,7 +3935,7 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -3935,13 +3944,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1">
         <v>200</v>
@@ -3949,7 +3958,7 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1">
         <v>10</v>
@@ -3958,13 +3967,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="1">
         <v>200</v>
@@ -3972,7 +3981,7 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -3981,13 +3990,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" s="1">
         <v>200</v>
@@ -3995,7 +4004,7 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1">
         <v>150</v>
@@ -4004,13 +4013,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="1">
         <v>200</v>
@@ -4018,7 +4027,7 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="1">
         <v>500</v>
@@ -4027,13 +4036,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G7" s="1">
         <v>200</v>
@@ -4041,7 +4050,7 @@
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="7">
         <v>1500</v>
@@ -4050,13 +4059,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="1">
         <v>200</v>
@@ -4064,7 +4073,7 @@
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="1">
         <v>0.1</v>
@@ -4073,13 +4082,13 @@
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9" s="1">
         <v>200</v>
@@ -4087,7 +4096,7 @@
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -4096,13 +4105,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="1">
         <v>200</v>
@@ -4110,7 +4119,7 @@
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B11" s="1">
         <v>10</v>
@@ -4119,13 +4128,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G11" s="1">
         <v>200</v>
@@ -4133,7 +4142,7 @@
     </row>
     <row r="12" spans="1:7" ht="20" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B12" s="1">
         <v>50</v>
@@ -4142,13 +4151,13 @@
         <v>11</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G12" s="1">
         <v>200</v>
@@ -4156,7 +4165,7 @@
     </row>
     <row r="13" spans="1:7" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="1">
         <v>150</v>
@@ -4165,13 +4174,13 @@
         <v>12</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="1">
         <v>10</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="1">
         <v>200</v>
@@ -4179,7 +4188,7 @@
     </row>
     <row r="14" spans="1:7" ht="20" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="1">
         <v>500</v>
@@ -4188,13 +4197,13 @@
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1">
         <v>10</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G14" s="1">
         <v>200</v>
@@ -4202,7 +4211,7 @@
     </row>
     <row r="15" spans="1:7" ht="20" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="7">
         <v>1500</v>
@@ -4211,13 +4220,13 @@
         <v>14</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1">
         <v>10</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G15" s="1">
         <v>200</v>
@@ -4225,7 +4234,7 @@
     </row>
     <row r="16" spans="1:7" ht="20" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" s="1">
         <v>0.1</v>
@@ -4234,13 +4243,13 @@
         <v>15</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E16" s="1">
         <v>10</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1">
         <v>200</v>
@@ -4248,7 +4257,7 @@
     </row>
     <row r="17" spans="1:7" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" s="1">
         <v>2</v>
@@ -4257,13 +4266,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E17" s="1">
         <v>10</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="1">
         <v>200</v>
@@ -4271,7 +4280,7 @@
     </row>
     <row r="18" spans="1:7" ht="20" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="1">
         <v>10</v>
@@ -4280,13 +4289,13 @@
         <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="1">
         <v>10</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G18" s="1">
         <v>200</v>
@@ -4294,7 +4303,7 @@
     </row>
     <row r="19" spans="1:7" ht="20" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="1">
         <v>50</v>
@@ -4303,13 +4312,13 @@
         <v>18</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="1">
         <v>10</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G19" s="1">
         <v>200</v>
@@ -4317,7 +4326,7 @@
     </row>
     <row r="20" spans="1:7" ht="20" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B20" s="1">
         <v>150</v>
@@ -4326,13 +4335,13 @@
         <v>19</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1">
         <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G20" s="1">
         <v>200</v>
@@ -4340,7 +4349,7 @@
     </row>
     <row r="21" spans="1:7" ht="20" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21" s="1">
         <v>500</v>
@@ -4349,13 +4358,13 @@
         <v>20</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="1">
         <v>10</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G21" s="1">
         <v>200</v>
@@ -4363,7 +4372,7 @@
     </row>
     <row r="22" spans="1:7" ht="20" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="7">
         <v>1500</v>
@@ -4372,13 +4381,13 @@
         <v>21</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="1">
         <v>10</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="1">
         <v>200</v>
@@ -4386,7 +4395,7 @@
     </row>
     <row r="23" spans="1:7" ht="20" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="1">
         <v>0.3</v>
@@ -4395,13 +4404,13 @@
         <v>22</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="1">
         <v>10</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G23" s="1">
         <v>200</v>
@@ -4409,7 +4418,7 @@
     </row>
     <row r="24" spans="1:7" ht="20" customHeight="1">
       <c r="A24" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
@@ -4418,13 +4427,13 @@
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E24" s="1">
         <v>10</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G24" s="1">
         <v>200</v>
@@ -4432,7 +4441,7 @@
     </row>
     <row r="25" spans="1:7" ht="20" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B25" s="1">
         <v>30</v>
@@ -4441,13 +4450,13 @@
         <v>24</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1">
         <v>10</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G25" s="1">
         <v>200</v>
@@ -4455,7 +4464,7 @@
     </row>
     <row r="26" spans="1:7" ht="20" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B26" s="1">
         <v>150</v>
@@ -4464,13 +4473,13 @@
         <v>25</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1">
         <v>10</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G26" s="1">
         <v>200</v>
@@ -4478,7 +4487,7 @@
     </row>
     <row r="27" spans="1:7" ht="20" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" s="1">
         <v>500</v>
@@ -4487,13 +4496,13 @@
         <v>26</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="1">
         <v>10</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G27" s="1">
         <v>200</v>
@@ -4501,7 +4510,7 @@
     </row>
     <row r="28" spans="1:7" ht="20" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B28" s="1">
         <v>1500</v>
@@ -4510,13 +4519,13 @@
         <v>27</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E28" s="1">
         <v>10</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G28" s="1">
         <v>200</v>
@@ -4524,7 +4533,7 @@
     </row>
     <row r="29" spans="1:7" ht="20" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B29" s="7">
         <v>4500</v>
@@ -4533,13 +4542,13 @@
         <v>28</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29" s="1">
         <v>10</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G29" s="1">
         <v>200</v>
@@ -4547,7 +4556,7 @@
     </row>
     <row r="30" spans="1:7" ht="20" customHeight="1">
       <c r="A30" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B30" s="1">
         <v>0.3</v>
@@ -4556,13 +4565,13 @@
         <v>29</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E30" s="1">
         <v>10</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G30" s="1">
         <v>200</v>
@@ -4570,7 +4579,7 @@
     </row>
     <row r="31" spans="1:7" ht="20" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B31" s="1">
         <v>3</v>
@@ -4579,13 +4588,13 @@
         <v>30</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E31" s="1">
         <v>10</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" s="1">
         <v>200</v>
@@ -4593,7 +4602,7 @@
     </row>
     <row r="32" spans="1:7" ht="20" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32" s="1">
         <v>15</v>
@@ -4602,13 +4611,13 @@
         <v>31</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E32" s="1">
         <v>10</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G32" s="1">
         <v>200</v>
@@ -4616,7 +4625,7 @@
     </row>
     <row r="33" spans="1:7" ht="20" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="1">
         <v>50</v>
@@ -4625,13 +4634,13 @@
         <v>32</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E33" s="1">
         <v>10</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G33" s="1">
         <v>200</v>
@@ -4639,7 +4648,7 @@
     </row>
     <row r="34" spans="1:7" ht="20" customHeight="1">
       <c r="A34" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="1">
         <v>200</v>
@@ -4648,13 +4657,13 @@
         <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="1">
         <v>10</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G34" s="1">
         <v>200</v>
@@ -4662,7 +4671,7 @@
     </row>
     <row r="35" spans="1:7" ht="20" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="1">
         <v>600</v>
@@ -4671,13 +4680,13 @@
         <v>34</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E35" s="1">
         <v>10</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G35" s="1">
         <v>200</v>
@@ -4685,7 +4694,7 @@
     </row>
     <row r="36" spans="1:7" ht="20" customHeight="1">
       <c r="A36" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B36" s="7">
         <v>7</v>
@@ -4694,13 +4703,13 @@
         <v>35</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" s="1">
         <v>10</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G36" s="1">
         <v>200</v>
@@ -4708,7 +4717,7 @@
     </row>
     <row r="37" spans="1:7" ht="20" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B37" s="7">
         <v>30</v>
@@ -4717,13 +4726,13 @@
         <v>36</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E37" s="1">
         <v>10</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G37" s="1">
         <v>200</v>
@@ -4731,7 +4740,7 @@
     </row>
     <row r="38" spans="1:7" ht="20" customHeight="1">
       <c r="A38" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B38" s="1">
         <v>90</v>
@@ -4740,13 +4749,13 @@
         <v>37</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E38" s="1">
         <v>10</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G38" s="1">
         <v>200</v>
@@ -4754,7 +4763,7 @@
     </row>
     <row r="39" spans="1:7" ht="20" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B39" s="1">
         <v>250</v>
@@ -4763,13 +4772,13 @@
         <v>38</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E39" s="1">
         <v>10</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G39" s="1">
         <v>200</v>
@@ -4843,27 +4852,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="20" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -4872,13 +4881,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E2" s="1">
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="1">
         <v>200</v>
@@ -4886,7 +4895,7 @@
     </row>
     <row r="3" spans="1:7" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -4895,13 +4904,13 @@
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="1">
         <v>200</v>
@@ -4909,7 +4918,7 @@
     </row>
     <row r="4" spans="1:7" ht="20" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="1">
         <v>15</v>
@@ -4918,13 +4927,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="1">
         <v>200</v>
@@ -4932,7 +4941,7 @@
     </row>
     <row r="5" spans="1:7" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" s="1">
         <v>60</v>
@@ -4941,13 +4950,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1">
         <v>10</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5" s="1">
         <v>200</v>
@@ -4955,7 +4964,7 @@
     </row>
     <row r="6" spans="1:7" ht="20" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" s="1">
         <v>180</v>
@@ -4964,13 +4973,13 @@
         <v>5</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="1">
         <v>200</v>
@@ -4978,7 +4987,7 @@
     </row>
     <row r="7" spans="1:7" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1">
         <v>480</v>
@@ -4987,13 +4996,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1">
         <v>10</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G7" s="1">
         <v>200</v>
@@ -5001,7 +5010,7 @@
     </row>
     <row r="8" spans="1:7" ht="20" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="7">
         <v>900</v>
@@ -5010,13 +5019,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="1">
         <v>10</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="1">
         <v>200</v>
@@ -5024,7 +5033,7 @@
     </row>
     <row r="9" spans="1:7" ht="20" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" s="1">
         <v>1440</v>
@@ -5033,13 +5042,13 @@
         <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9" s="1">
         <v>200</v>
@@ -5047,7 +5056,7 @@
     </row>
     <row r="10" spans="1:7" ht="20" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B10" s="1">
         <v>0.25</v>
@@ -5056,13 +5065,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="1">
         <v>200</v>
@@ -5070,7 +5079,7 @@
     </row>
     <row r="11" spans="1:7" ht="20" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="1">
         <v>0.5</v>
@@ -5079,13 +5088,13 @@
         <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1">
         <v>10</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G11" s="1">
         <v>200</v>

</xml_diff>

<commit_message>
dev of item system
</commit_message>
<xml_diff>
--- a/gameData/shared/Items.xlsx
+++ b/gameData/shared/Items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9760" yWindow="3160" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="4"/>
+    <workbookView xWindow="11300" yWindow="2820" windowWidth="25600" windowHeight="16060" tabRatio="883" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="special" sheetId="2" r:id="rId1"/>
@@ -832,7 +832,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="394">
+  <cellStyleXfs count="414">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -847,6 +847,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1262,7 +1282,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="394">
+  <cellStyles count="414">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1462,6 +1482,16 @@
     <cellStyle name="超链接" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="390" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="412" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1654,6 +1684,16 @@
     <cellStyle name="访问过的超链接" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="391" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="413" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -3079,8 +3119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4538,8 +4578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -4556,7 +4596,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>194</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>40</v>
@@ -5499,7 +5539,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -5883,8 +5923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>